<commit_message>
Partially finished error table
</commit_message>
<xml_diff>
--- a/lu_hs_g.xlsx
+++ b/lu_hs_g.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>LU</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Givens</t>
+  </si>
+  <si>
+    <t>LU - LU - H</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
                   <c:v>2.7800000000000003E-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.7800000000000003E-17</c:v>
+                  <c:v>2.7800000000000003E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.2500000000000005E-17</c:v>
@@ -304,7 +307,7 @@
                   <c:v>5.3099999999999995E-16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0000000000000002E-15</c:v>
+                  <c:v>2.0099999999999999E-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.2100000000000001E-15</c:v>
@@ -623,7 +626,7 @@
                   <c:v>5.5500000000000002E-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.7800000000000003E-17</c:v>
+                  <c:v>2.7800000000000003E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.8399999999999998E-16</c:v>
@@ -689,11 +692,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="331186768"/>
-        <c:axId val="331187944"/>
+        <c:axId val="253474048"/>
+        <c:axId val="253474440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="331186768"/>
+        <c:axId val="253474048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -781,12 +784,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331187944"/>
+        <c:crossAx val="253474440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="331187944"/>
+        <c:axId val="253474440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331186768"/>
+        <c:crossAx val="253474048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1081,7 +1084,7 @@
                   <c:v>2.7800000000000003E-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.7800000000000003E-17</c:v>
+                  <c:v>2.7800000000000003E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.2500000000000005E-17</c:v>
@@ -1090,7 +1093,7 @@
                   <c:v>5.3099999999999995E-16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0000000000000002E-15</c:v>
+                  <c:v>2.0099999999999999E-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.2100000000000001E-15</c:v>
@@ -1409,7 +1412,7 @@
                   <c:v>5.5500000000000002E-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.7800000000000003E-17</c:v>
+                  <c:v>2.7800000000000003E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.8399999999999998E-16</c:v>
@@ -1475,11 +1478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429303776"/>
-        <c:axId val="429304168"/>
+        <c:axId val="253466992"/>
+        <c:axId val="253468560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429303776"/>
+        <c:axId val="253466992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,12 +1539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="429304168"/>
+        <c:crossAx val="253468560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429304168"/>
+        <c:axId val="253468560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1598,7 +1601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="429303776"/>
+        <c:crossAx val="253466992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2763,16 +2766,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3148,15 +3151,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3166,8 +3169,17 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3180,22 +3192,40 @@
       <c r="D3" s="1">
         <v>5.5500000000000002E-17</v>
       </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.2200000000000001E-16</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>-2.7800000000000003E-17</v>
+        <v>2.7800000000000003E-17</v>
       </c>
       <c r="C4" s="1">
         <v>8.3300000000000005E-17</v>
       </c>
       <c r="D4" s="1">
-        <v>-2.7800000000000003E-17</v>
+        <v>2.7800000000000003E-17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6.6599999999999998E-16</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3208,8 +3238,17 @@
       <c r="D5" s="1">
         <v>2.8399999999999998E-16</v>
       </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6.6599999999999998E-16</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3222,13 +3261,22 @@
       <c r="D6" s="1">
         <v>8.6699999999999996E-17</v>
       </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.11E-16</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.3900000000000002E-17</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2.0000000000000002E-15</v>
+        <v>2.0099999999999999E-15</v>
       </c>
       <c r="C7" s="1">
         <v>3.3399999999999998E-15</v>
@@ -3236,8 +3284,17 @@
       <c r="D7" s="1">
         <v>6.7299999999999999E-16</v>
       </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.6599999999999998E-16</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.3900000000000002E-17</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3251,7 +3308,7 @@
         <v>1.21E-14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3265,7 +3322,7 @@
         <v>7.62E-15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3279,7 +3336,7 @@
         <v>1.8200000000000001E-13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3293,7 +3350,7 @@
         <v>9.89E-14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3307,7 +3364,7 @@
         <v>2.7000000000000001E-13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3321,7 +3378,7 @@
         <v>8.2800000000000001E-13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3335,7 +3392,7 @@
         <v>1.24E-11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3349,7 +3406,7 @@
         <v>1.78E-13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>